<commit_message>
Getting a singular B matrix
</commit_message>
<xml_diff>
--- a/data/case12.xlsx
+++ b/data/case12.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -1050,7 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1473,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,6 +2063,71 @@
         <v>0</v>
       </c>
       <c r="U9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
case12 Correct Line 5 (to-from)
</commit_message>
<xml_diff>
--- a/data/case12.xlsx
+++ b/data/case12.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -1050,7 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -2141,8 +2141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,7 +2331,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>0</v>

</xml_diff>

<commit_message>
Downloaded old root to correct DCPF
PGIA-Model-432b84e5fc13780f8fc431102033968fe66d64a2
</commit_message>
<xml_diff>
--- a/data/case12.xlsx
+++ b/data/case12.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\PGIA-Model\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\PGIA-Model-432b84e5fc13780f8fc431102033968fe66d64a2\PGIA-Model-432b84e5fc13780f8fc431102033968fe66d64a2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13740" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="7125" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -1473,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:U10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,71 +2063,6 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
         <v>0</v>
       </c>
     </row>
@@ -2142,7 +2077,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
funcSolar Added (no dist)
</commit_message>
<xml_diff>
--- a/data/case12.xlsx
+++ b/data/case12.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\PGIA-Model-432b84e5fc13780f8fc431102033968fe66d64a2\PGIA-Model-432b84e5fc13780f8fc431102033968fe66d64a2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\PGIA-Model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="7125" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5595" windowHeight="5220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -1473,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,6 +2063,71 @@
         <v>0</v>
       </c>
       <c r="U9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
         <v>0</v>
       </c>
     </row>
@@ -2076,7 +2141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Model Convergence Test
</commit_message>
<xml_diff>
--- a/data/case12.xlsx
+++ b/data/case12.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5595" windowHeight="5220" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5595" windowHeight="5220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,34 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alejandro Palomino</author>
+  </authors>
+  <commentList>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">sBase 100 kVA
+ 100000 VA
+vBase 240 V
+iBase 416.6667 
+zBase 0.576 
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Alejandro Palomino</author>
@@ -43,7 +71,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Alejandro Palomino</author>
@@ -53,12 +81,44 @@
       <text>
         <r>
           <rPr>
+            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Per-Unit Reactance</t>
+          <t xml:space="preserve">Per-Unit Reactance
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sweetbriar has resistance of</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0.101 / 1000ft. Assume 125ft per cable = 0.012625
+zBase = 0.576
+pu_X = 0.012625/zBase = 0.02192</t>
         </r>
       </text>
     </comment>
@@ -96,9 +156,6 @@
     <t>Va</t>
   </si>
   <si>
-    <t>baseKV</t>
-  </si>
-  <si>
     <t>zone</t>
   </si>
   <si>
@@ -208,13 +265,16 @@
   </si>
   <si>
     <t>line</t>
+  </si>
+  <si>
+    <t>baseV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,6 +410,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -1047,11 +1114,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,16 +1152,16 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1126,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>12.4</v>
+        <v>240</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1167,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>12.4</v>
+        <v>240</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -1208,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>12.4</v>
+        <v>240</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1249,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>12.4</v>
+        <v>240</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -1290,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>12.4</v>
+        <v>240</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -1331,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>12.4</v>
+        <v>240</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1372,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>12.4</v>
+        <v>240</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1413,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>12.4</v>
+        <v>240</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1454,7 +1521,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>12.4</v>
+        <v>240</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1468,6 +1535,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1475,75 +1543,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>26</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>27</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>29</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>30</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>31</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>32</v>
-      </c>
-      <c r="U1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -2141,54 +2209,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>44</v>
-      </c>
-      <c r="N1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2205,7 +2273,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1.055E-2</v>
+        <v>2.1919999999999999E-2</v>
       </c>
       <c r="F2">
         <v>0.10249999999999999</v>
@@ -2249,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1.055E-2</v>
+        <v>2.1919999999999999E-2</v>
       </c>
       <c r="F3">
         <v>7.7499999999999999E-2</v>
@@ -2293,7 +2361,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1.055E-2</v>
+        <v>2.1919999999999999E-2</v>
       </c>
       <c r="F4">
         <v>7.7499999999999999E-2</v>
@@ -2337,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1.055E-2</v>
+        <v>2.1919999999999999E-2</v>
       </c>
       <c r="F5">
         <v>7.7499999999999999E-2</v>
@@ -2381,7 +2449,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1.055E-2</v>
+        <v>2.1919999999999999E-2</v>
       </c>
       <c r="F6">
         <v>7.7499999999999999E-2</v>
@@ -2425,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1.055E-2</v>
+        <v>2.1919999999999999E-2</v>
       </c>
       <c r="F7">
         <v>7.7499999999999999E-2</v>
@@ -2469,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1.055E-2</v>
+        <v>2.1919999999999999E-2</v>
       </c>
       <c r="F8">
         <v>7.7499999999999999E-2</v>
@@ -2513,7 +2581,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1.055E-2</v>
+        <v>2.1919999999999999E-2</v>
       </c>
       <c r="F9">
         <v>7.7499999999999999E-2</v>
@@ -2545,6 +2613,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>